<commit_message>
Eliminated empty columns and fixed codes
</commit_message>
<xml_diff>
--- a/source_data_old/02_data.xlsx
+++ b/source_data_old/02_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\gender_data_portal\source_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gonzalezmorales\projects\ARCGIS HUBS\gender_data_portal\source_data_old\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{ECEAF5B7-0416-4CCD-A6CA-BAB7E74F3A63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B5521C5-E096-43C1-8032-3EF10EC2EFF6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D791385-7735-4459-958F-B979FAFF47B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1141,7 +1141,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1984,7 +1984,7 @@
       <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
@@ -1997,7 +1997,7 @@
     <col min="28" max="28" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2083,7 +2083,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:28">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -2169,7 +2169,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="3" spans="1:28">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2255,7 +2255,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="4" spans="1:28">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2341,7 +2341,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="5" spans="1:28">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -2427,7 +2427,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="6" spans="1:28">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -2513,7 +2513,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="7" spans="1:28">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -2599,7 +2599,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="8" spans="1:28">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -2685,7 +2685,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="9" spans="1:28">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -2771,7 +2771,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="10" spans="1:28">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
@@ -2857,7 +2857,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="11" spans="1:28">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2</v>
       </c>
@@ -2943,7 +2943,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="12" spans="1:28">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2</v>
       </c>
@@ -3029,7 +3029,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="13" spans="1:28">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
@@ -3115,7 +3115,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="14" spans="1:28">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2</v>
       </c>
@@ -3201,7 +3201,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="15" spans="1:28">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
@@ -3287,7 +3287,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="16" spans="1:28">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
@@ -3373,7 +3373,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="17" spans="1:28">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2</v>
       </c>
@@ -3459,7 +3459,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="18" spans="1:28">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2</v>
       </c>
@@ -3545,7 +3545,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="19" spans="1:28">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2</v>
       </c>
@@ -3631,7 +3631,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="20" spans="1:28">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2</v>
       </c>
@@ -3717,7 +3717,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="21" spans="1:28">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2</v>
       </c>
@@ -3803,7 +3803,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="22" spans="1:28">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2</v>
       </c>
@@ -3889,7 +3889,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="23" spans="1:28">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2</v>
       </c>
@@ -3975,7 +3975,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="24" spans="1:28">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2</v>
       </c>
@@ -4061,7 +4061,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="25" spans="1:28">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2</v>
       </c>
@@ -4147,7 +4147,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="26" spans="1:28">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2</v>
       </c>
@@ -4233,7 +4233,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="27" spans="1:28">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2</v>
       </c>
@@ -4319,7 +4319,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="28" spans="1:28">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2</v>
       </c>
@@ -4405,7 +4405,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="29" spans="1:28">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2</v>
       </c>
@@ -4491,7 +4491,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="30" spans="1:28">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2</v>
       </c>
@@ -4577,7 +4577,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="31" spans="1:28">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2</v>
       </c>
@@ -4663,7 +4663,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="32" spans="1:28">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2</v>
       </c>
@@ -4749,7 +4749,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="33" spans="1:28">
+    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2</v>
       </c>
@@ -4835,7 +4835,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="34" spans="1:28">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2</v>
       </c>
@@ -4921,7 +4921,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="35" spans="1:28">
+    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2</v>
       </c>
@@ -5007,7 +5007,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="36" spans="1:28">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2</v>
       </c>
@@ -5093,7 +5093,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="37" spans="1:28">
+    <row r="37" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2</v>
       </c>
@@ -5179,7 +5179,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="38" spans="1:28">
+    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2</v>
       </c>
@@ -5265,7 +5265,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="39" spans="1:28">
+    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2</v>
       </c>
@@ -5351,7 +5351,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="40" spans="1:28">
+    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2</v>
       </c>
@@ -5437,7 +5437,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="41" spans="1:28">
+    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2</v>
       </c>
@@ -5523,7 +5523,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="42" spans="1:28">
+    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2</v>
       </c>
@@ -5609,7 +5609,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="43" spans="1:28">
+    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2</v>
       </c>
@@ -5695,7 +5695,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="44" spans="1:28">
+    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2</v>
       </c>
@@ -5781,7 +5781,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="45" spans="1:28">
+    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2</v>
       </c>
@@ -5867,7 +5867,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="46" spans="1:28">
+    <row r="46" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2</v>
       </c>
@@ -5953,7 +5953,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="47" spans="1:28">
+    <row r="47" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2</v>
       </c>
@@ -6039,7 +6039,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="48" spans="1:28">
+    <row r="48" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2</v>
       </c>
@@ -6125,7 +6125,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="49" spans="1:28">
+    <row r="49" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2</v>
       </c>
@@ -6211,7 +6211,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="50" spans="1:28">
+    <row r="50" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2</v>
       </c>
@@ -6297,7 +6297,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="51" spans="1:28">
+    <row r="51" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2</v>
       </c>
@@ -6383,7 +6383,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="52" spans="1:28">
+    <row r="52" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2</v>
       </c>
@@ -6469,7 +6469,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="53" spans="1:28">
+    <row r="53" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2</v>
       </c>
@@ -6555,7 +6555,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="54" spans="1:28">
+    <row r="54" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2</v>
       </c>
@@ -6641,7 +6641,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="55" spans="1:28">
+    <row r="55" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2</v>
       </c>
@@ -6727,7 +6727,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="56" spans="1:28">
+    <row r="56" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2</v>
       </c>
@@ -6813,7 +6813,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="57" spans="1:28">
+    <row r="57" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2</v>
       </c>
@@ -6899,7 +6899,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="58" spans="1:28">
+    <row r="58" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2</v>
       </c>
@@ -6985,7 +6985,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="59" spans="1:28">
+    <row r="59" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2</v>
       </c>
@@ -7071,7 +7071,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="60" spans="1:28">
+    <row r="60" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2</v>
       </c>
@@ -7157,7 +7157,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="61" spans="1:28">
+    <row r="61" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>2</v>
       </c>
@@ -7243,7 +7243,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="62" spans="1:28">
+    <row r="62" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2</v>
       </c>
@@ -7329,7 +7329,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="63" spans="1:28">
+    <row r="63" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>2</v>
       </c>
@@ -7415,7 +7415,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="64" spans="1:28">
+    <row r="64" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>2</v>
       </c>
@@ -7501,7 +7501,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="65" spans="1:28">
+    <row r="65" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>2</v>
       </c>
@@ -7587,7 +7587,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="66" spans="1:28">
+    <row r="66" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>2</v>
       </c>
@@ -7673,7 +7673,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="67" spans="1:28">
+    <row r="67" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>2</v>
       </c>
@@ -7759,7 +7759,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="68" spans="1:28">
+    <row r="68" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>2</v>
       </c>
@@ -7845,7 +7845,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="69" spans="1:28">
+    <row r="69" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>2</v>
       </c>
@@ -7931,7 +7931,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="70" spans="1:28">
+    <row r="70" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>2</v>
       </c>
@@ -8017,7 +8017,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="71" spans="1:28">
+    <row r="71" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>2</v>
       </c>
@@ -8103,7 +8103,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="72" spans="1:28">
+    <row r="72" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>2</v>
       </c>
@@ -8189,7 +8189,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="73" spans="1:28">
+    <row r="73" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>2</v>
       </c>
@@ -8275,7 +8275,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="74" spans="1:28">
+    <row r="74" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>2</v>
       </c>
@@ -8361,7 +8361,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="75" spans="1:28">
+    <row r="75" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>2</v>
       </c>
@@ -8447,7 +8447,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="76" spans="1:28">
+    <row r="76" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>2</v>
       </c>
@@ -8533,7 +8533,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="77" spans="1:28">
+    <row r="77" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>2</v>
       </c>
@@ -8619,7 +8619,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="78" spans="1:28">
+    <row r="78" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>2</v>
       </c>
@@ -8705,7 +8705,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="79" spans="1:28">
+    <row r="79" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>2</v>
       </c>
@@ -8791,7 +8791,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="80" spans="1:28">
+    <row r="80" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>2</v>
       </c>
@@ -8877,7 +8877,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="81" spans="1:28">
+    <row r="81" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>2</v>
       </c>
@@ -8963,7 +8963,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="82" spans="1:28">
+    <row r="82" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>2</v>
       </c>
@@ -9049,7 +9049,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="83" spans="1:28">
+    <row r="83" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>2</v>
       </c>
@@ -9135,7 +9135,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="84" spans="1:28">
+    <row r="84" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>2</v>
       </c>
@@ -9221,7 +9221,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="85" spans="1:28">
+    <row r="85" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>2</v>
       </c>
@@ -9307,7 +9307,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="86" spans="1:28">
+    <row r="86" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>2</v>
       </c>
@@ -9393,7 +9393,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="87" spans="1:28">
+    <row r="87" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>2</v>
       </c>
@@ -9479,7 +9479,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="88" spans="1:28">
+    <row r="88" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>2</v>
       </c>
@@ -9565,7 +9565,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="89" spans="1:28">
+    <row r="89" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>2</v>
       </c>
@@ -9651,7 +9651,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="90" spans="1:28">
+    <row r="90" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>2</v>
       </c>
@@ -9737,7 +9737,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="91" spans="1:28">
+    <row r="91" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>2</v>
       </c>
@@ -9823,7 +9823,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="92" spans="1:28">
+    <row r="92" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>2</v>
       </c>
@@ -9909,7 +9909,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="93" spans="1:28">
+    <row r="93" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>2</v>
       </c>
@@ -9995,7 +9995,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="94" spans="1:28">
+    <row r="94" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>2</v>
       </c>
@@ -10081,7 +10081,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="95" spans="1:28">
+    <row r="95" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>2</v>
       </c>
@@ -10167,7 +10167,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="96" spans="1:28">
+    <row r="96" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>2</v>
       </c>
@@ -10253,7 +10253,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="97" spans="1:28">
+    <row r="97" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>2</v>
       </c>
@@ -10339,7 +10339,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="98" spans="1:28">
+    <row r="98" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>2</v>
       </c>
@@ -10425,7 +10425,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="99" spans="1:28">
+    <row r="99" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>2</v>
       </c>
@@ -10511,7 +10511,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="100" spans="1:28">
+    <row r="100" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>2</v>
       </c>
@@ -10597,7 +10597,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="101" spans="1:28">
+    <row r="101" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>2</v>
       </c>
@@ -10683,7 +10683,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="102" spans="1:28">
+    <row r="102" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>2</v>
       </c>
@@ -10769,7 +10769,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="103" spans="1:28">
+    <row r="103" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>2</v>
       </c>
@@ -10855,7 +10855,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="104" spans="1:28">
+    <row r="104" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>2</v>
       </c>
@@ -10941,7 +10941,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="105" spans="1:28">
+    <row r="105" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>2</v>
       </c>
@@ -11027,7 +11027,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="106" spans="1:28">
+    <row r="106" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>2</v>
       </c>
@@ -11113,7 +11113,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="107" spans="1:28">
+    <row r="107" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>2</v>
       </c>
@@ -11199,7 +11199,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="108" spans="1:28">
+    <row r="108" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>2</v>
       </c>
@@ -11285,7 +11285,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="109" spans="1:28">
+    <row r="109" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>2</v>
       </c>
@@ -11371,7 +11371,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="110" spans="1:28">
+    <row r="110" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>2</v>
       </c>
@@ -11457,7 +11457,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="111" spans="1:28">
+    <row r="111" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>2</v>
       </c>
@@ -11543,7 +11543,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="112" spans="1:28">
+    <row r="112" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>2</v>
       </c>
@@ -11629,7 +11629,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="113" spans="1:28">
+    <row r="113" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>2</v>
       </c>
@@ -11715,7 +11715,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="114" spans="1:28">
+    <row r="114" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>2</v>
       </c>
@@ -11801,7 +11801,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="115" spans="1:28">
+    <row r="115" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>2</v>
       </c>
@@ -11887,7 +11887,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="116" spans="1:28">
+    <row r="116" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>2</v>
       </c>
@@ -11973,7 +11973,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="117" spans="1:28">
+    <row r="117" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>2</v>
       </c>
@@ -12059,7 +12059,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="118" spans="1:28">
+    <row r="118" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>2</v>
       </c>
@@ -12145,7 +12145,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="119" spans="1:28">
+    <row r="119" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>2</v>
       </c>
@@ -12231,7 +12231,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="120" spans="1:28">
+    <row r="120" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>2</v>
       </c>
@@ -12317,7 +12317,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="121" spans="1:28">
+    <row r="121" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>2</v>
       </c>
@@ -12403,7 +12403,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="122" spans="1:28">
+    <row r="122" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>2</v>
       </c>
@@ -12489,7 +12489,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="123" spans="1:28">
+    <row r="123" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>2</v>
       </c>
@@ -12575,7 +12575,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="124" spans="1:28">
+    <row r="124" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>2</v>
       </c>
@@ -12661,7 +12661,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="125" spans="1:28">
+    <row r="125" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>2</v>
       </c>
@@ -12747,7 +12747,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="126" spans="1:28">
+    <row r="126" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>2</v>
       </c>
@@ -12833,7 +12833,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="127" spans="1:28">
+    <row r="127" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>2</v>
       </c>
@@ -12919,7 +12919,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="128" spans="1:28">
+    <row r="128" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>2</v>
       </c>
@@ -13005,7 +13005,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="129" spans="1:28">
+    <row r="129" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>2</v>
       </c>
@@ -13091,7 +13091,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="130" spans="1:28">
+    <row r="130" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>2</v>
       </c>
@@ -13177,7 +13177,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="131" spans="1:28">
+    <row r="131" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>2</v>
       </c>
@@ -13263,7 +13263,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="132" spans="1:28">
+    <row r="132" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>2</v>
       </c>
@@ -13349,7 +13349,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="133" spans="1:28">
+    <row r="133" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>2</v>
       </c>
@@ -13435,7 +13435,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="134" spans="1:28">
+    <row r="134" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>2</v>
       </c>
@@ -13521,7 +13521,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="135" spans="1:28">
+    <row r="135" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>2</v>
       </c>
@@ -13607,7 +13607,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="136" spans="1:28">
+    <row r="136" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>2</v>
       </c>
@@ -13693,7 +13693,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="137" spans="1:28">
+    <row r="137" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>2</v>
       </c>
@@ -13779,7 +13779,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="138" spans="1:28">
+    <row r="138" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>2</v>
       </c>
@@ -13865,7 +13865,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="139" spans="1:28">
+    <row r="139" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>2</v>
       </c>
@@ -13951,7 +13951,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="140" spans="1:28">
+    <row r="140" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>2</v>
       </c>
@@ -14037,7 +14037,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="141" spans="1:28">
+    <row r="141" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>2</v>
       </c>
@@ -14123,7 +14123,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="142" spans="1:28">
+    <row r="142" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>2</v>
       </c>
@@ -14209,7 +14209,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="143" spans="1:28">
+    <row r="143" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>2</v>
       </c>
@@ -14295,7 +14295,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="144" spans="1:28">
+    <row r="144" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>2</v>
       </c>
@@ -14381,7 +14381,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="145" spans="1:28">
+    <row r="145" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>2</v>
       </c>
@@ -14467,7 +14467,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="146" spans="1:28">
+    <row r="146" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>2</v>
       </c>
@@ -14553,7 +14553,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="147" spans="1:28">
+    <row r="147" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>2</v>
       </c>
@@ -14639,7 +14639,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="148" spans="1:28">
+    <row r="148" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>2</v>
       </c>
@@ -14725,7 +14725,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="149" spans="1:28">
+    <row r="149" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>2</v>
       </c>
@@ -14811,7 +14811,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="150" spans="1:28">
+    <row r="150" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>2</v>
       </c>
@@ -14897,7 +14897,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="151" spans="1:28">
+    <row r="151" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>2</v>
       </c>
@@ -14983,7 +14983,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="152" spans="1:28">
+    <row r="152" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>2</v>
       </c>
@@ -15069,7 +15069,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="153" spans="1:28">
+    <row r="153" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>2</v>
       </c>
@@ -15155,7 +15155,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="154" spans="1:28">
+    <row r="154" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>2</v>
       </c>
@@ -15241,7 +15241,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="155" spans="1:28">
+    <row r="155" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>2</v>
       </c>
@@ -15327,7 +15327,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="156" spans="1:28">
+    <row r="156" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>2</v>
       </c>
@@ -15413,7 +15413,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="157" spans="1:28">
+    <row r="157" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>2</v>
       </c>
@@ -15499,7 +15499,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="158" spans="1:28">
+    <row r="158" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>2</v>
       </c>
@@ -15585,7 +15585,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="159" spans="1:28">
+    <row r="159" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>2</v>
       </c>
@@ -15671,7 +15671,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="160" spans="1:28">
+    <row r="160" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>2</v>
       </c>
@@ -15757,7 +15757,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="161" spans="1:28">
+    <row r="161" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>2</v>
       </c>
@@ -15843,7 +15843,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="162" spans="1:28">
+    <row r="162" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>2</v>
       </c>
@@ -15929,7 +15929,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="163" spans="1:28">
+    <row r="163" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>2</v>
       </c>
@@ -16015,7 +16015,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="164" spans="1:28">
+    <row r="164" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>2</v>
       </c>
@@ -16101,7 +16101,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="165" spans="1:28">
+    <row r="165" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>2</v>
       </c>
@@ -16187,7 +16187,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="166" spans="1:28">
+    <row r="166" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>2</v>
       </c>
@@ -16273,7 +16273,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="167" spans="1:28">
+    <row r="167" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>2</v>
       </c>
@@ -16359,7 +16359,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="168" spans="1:28">
+    <row r="168" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>2</v>
       </c>
@@ -16445,7 +16445,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="169" spans="1:28">
+    <row r="169" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>2</v>
       </c>
@@ -16531,7 +16531,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="170" spans="1:28">
+    <row r="170" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>2</v>
       </c>
@@ -16617,7 +16617,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="171" spans="1:28">
+    <row r="171" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>2</v>
       </c>
@@ -16703,7 +16703,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="172" spans="1:28">
+    <row r="172" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>2</v>
       </c>
@@ -16789,7 +16789,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="173" spans="1:28">
+    <row r="173" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>2</v>
       </c>
@@ -16875,7 +16875,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="174" spans="1:28">
+    <row r="174" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>2</v>
       </c>
@@ -16961,7 +16961,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="175" spans="1:28">
+    <row r="175" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>2</v>
       </c>
@@ -17047,7 +17047,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="176" spans="1:28">
+    <row r="176" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>2</v>
       </c>
@@ -17133,7 +17133,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="177" spans="1:28">
+    <row r="177" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>2</v>
       </c>
@@ -17219,7 +17219,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="178" spans="1:28">
+    <row r="178" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>2</v>
       </c>
@@ -17305,7 +17305,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="179" spans="1:28">
+    <row r="179" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>2</v>
       </c>
@@ -17391,7 +17391,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="180" spans="1:28">
+    <row r="180" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>2</v>
       </c>
@@ -17477,7 +17477,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="181" spans="1:28">
+    <row r="181" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>2</v>
       </c>
@@ -17563,7 +17563,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="182" spans="1:28">
+    <row r="182" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>2</v>
       </c>
@@ -17649,7 +17649,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="183" spans="1:28">
+    <row r="183" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>2</v>
       </c>
@@ -17735,7 +17735,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="184" spans="1:28">
+    <row r="184" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>2</v>
       </c>
@@ -17821,7 +17821,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="185" spans="1:28">
+    <row r="185" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>2</v>
       </c>
@@ -17907,7 +17907,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="186" spans="1:28">
+    <row r="186" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>2</v>
       </c>
@@ -17993,7 +17993,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="187" spans="1:28">
+    <row r="187" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>2</v>
       </c>
@@ -18079,7 +18079,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="188" spans="1:28">
+    <row r="188" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>2</v>
       </c>
@@ -18165,7 +18165,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="189" spans="1:28">
+    <row r="189" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>2</v>
       </c>
@@ -18251,7 +18251,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="190" spans="1:28">
+    <row r="190" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>2</v>
       </c>
@@ -18337,7 +18337,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="191" spans="1:28">
+    <row r="191" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>2</v>
       </c>
@@ -18423,7 +18423,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="192" spans="1:28">
+    <row r="192" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>2</v>
       </c>
@@ -18509,7 +18509,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="193" spans="1:28">
+    <row r="193" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>2</v>
       </c>
@@ -18595,7 +18595,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="194" spans="1:28">
+    <row r="194" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>2</v>
       </c>
@@ -18681,7 +18681,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="195" spans="1:28">
+    <row r="195" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>2</v>
       </c>
@@ -18767,7 +18767,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="196" spans="1:28">
+    <row r="196" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>2</v>
       </c>
@@ -18853,7 +18853,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="197" spans="1:28">
+    <row r="197" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>2</v>
       </c>
@@ -18939,7 +18939,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="198" spans="1:28">
+    <row r="198" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>2</v>
       </c>
@@ -19025,7 +19025,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="199" spans="1:28">
+    <row r="199" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>2</v>
       </c>
@@ -19111,7 +19111,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="200" spans="1:28">
+    <row r="200" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>2</v>
       </c>
@@ -19197,7 +19197,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="201" spans="1:28">
+    <row r="201" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>2</v>
       </c>
@@ -19283,7 +19283,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="202" spans="1:28">
+    <row r="202" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>2</v>
       </c>
@@ -19369,7 +19369,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="203" spans="1:28">
+    <row r="203" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>2</v>
       </c>
@@ -19455,7 +19455,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="204" spans="1:28">
+    <row r="204" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>2</v>
       </c>
@@ -19541,7 +19541,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="205" spans="1:28">
+    <row r="205" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>2</v>
       </c>
@@ -19627,7 +19627,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="206" spans="1:28">
+    <row r="206" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>2</v>
       </c>
@@ -19713,7 +19713,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="207" spans="1:28">
+    <row r="207" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>2</v>
       </c>
@@ -19799,7 +19799,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="208" spans="1:28">
+    <row r="208" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>2</v>
       </c>
@@ -19885,7 +19885,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="209" spans="1:28">
+    <row r="209" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>2</v>
       </c>
@@ -19971,7 +19971,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="210" spans="1:28">
+    <row r="210" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>2</v>
       </c>
@@ -20057,7 +20057,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="211" spans="1:28">
+    <row r="211" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>2</v>
       </c>
@@ -20143,7 +20143,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="212" spans="1:28">
+    <row r="212" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>2</v>
       </c>
@@ -20229,7 +20229,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="213" spans="1:28">
+    <row r="213" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>2</v>
       </c>
@@ -20315,7 +20315,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="214" spans="1:28">
+    <row r="214" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>2</v>
       </c>
@@ -20401,7 +20401,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="215" spans="1:28">
+    <row r="215" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>2</v>
       </c>
@@ -20487,7 +20487,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="216" spans="1:28">
+    <row r="216" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>2</v>
       </c>
@@ -20573,7 +20573,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="217" spans="1:28">
+    <row r="217" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>2</v>
       </c>
@@ -20659,7 +20659,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="218" spans="1:28">
+    <row r="218" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>2</v>
       </c>
@@ -20745,7 +20745,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="219" spans="1:28">
+    <row r="219" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>2</v>
       </c>
@@ -20831,7 +20831,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="220" spans="1:28">
+    <row r="220" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>2</v>
       </c>
@@ -20917,7 +20917,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="221" spans="1:28">
+    <row r="221" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>2</v>
       </c>
@@ -21003,7 +21003,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="222" spans="1:28">
+    <row r="222" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>2</v>
       </c>
@@ -21089,7 +21089,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="223" spans="1:28">
+    <row r="223" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>2</v>
       </c>
@@ -21175,7 +21175,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="224" spans="1:28">
+    <row r="224" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>2</v>
       </c>
@@ -21261,7 +21261,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="225" spans="1:28">
+    <row r="225" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>2</v>
       </c>
@@ -21347,7 +21347,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="226" spans="1:28">
+    <row r="226" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>2</v>
       </c>
@@ -21433,7 +21433,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="227" spans="1:28">
+    <row r="227" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>2</v>
       </c>
@@ -21519,7 +21519,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="228" spans="1:28">
+    <row r="228" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>2</v>
       </c>
@@ -21605,7 +21605,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="229" spans="1:28">
+    <row r="229" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>2</v>
       </c>
@@ -21691,7 +21691,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="230" spans="1:28">
+    <row r="230" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>2</v>
       </c>
@@ -21777,7 +21777,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="231" spans="1:28">
+    <row r="231" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>2</v>
       </c>
@@ -21863,7 +21863,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="232" spans="1:28">
+    <row r="232" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>2</v>
       </c>
@@ -21949,7 +21949,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="233" spans="1:28">
+    <row r="233" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>2</v>
       </c>
@@ -22035,7 +22035,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="234" spans="1:28">
+    <row r="234" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>2</v>
       </c>
@@ -22121,7 +22121,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="235" spans="1:28">
+    <row r="235" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>2</v>
       </c>
@@ -22207,7 +22207,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="236" spans="1:28">
+    <row r="236" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>2</v>
       </c>
@@ -22293,7 +22293,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="237" spans="1:28">
+    <row r="237" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>2</v>
       </c>
@@ -22379,7 +22379,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="238" spans="1:28">
+    <row r="238" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>2</v>
       </c>
@@ -22465,7 +22465,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="239" spans="1:28">
+    <row r="239" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>2</v>
       </c>
@@ -22551,7 +22551,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="240" spans="1:28">
+    <row r="240" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>2</v>
       </c>
@@ -22637,7 +22637,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="241" spans="1:28">
+    <row r="241" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>2</v>
       </c>
@@ -22723,7 +22723,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="242" spans="1:28">
+    <row r="242" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>2</v>
       </c>
@@ -22809,7 +22809,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="243" spans="1:28">
+    <row r="243" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>2</v>
       </c>
@@ -22895,7 +22895,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="244" spans="1:28">
+    <row r="244" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>2</v>
       </c>
@@ -22981,7 +22981,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="245" spans="1:28">
+    <row r="245" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>2</v>
       </c>
@@ -23067,7 +23067,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="246" spans="1:28">
+    <row r="246" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>2</v>
       </c>
@@ -23153,7 +23153,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="247" spans="1:28">
+    <row r="247" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>2</v>
       </c>
@@ -23239,7 +23239,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="248" spans="1:28">
+    <row r="248" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>2</v>
       </c>
@@ -23325,7 +23325,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="249" spans="1:28">
+    <row r="249" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>2</v>
       </c>
@@ -23411,7 +23411,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="250" spans="1:28">
+    <row r="250" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>2</v>
       </c>
@@ -23497,7 +23497,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="251" spans="1:28">
+    <row r="251" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>2</v>
       </c>
@@ -23583,7 +23583,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="252" spans="1:28">
+    <row r="252" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>2</v>
       </c>
@@ -23669,7 +23669,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="253" spans="1:28">
+    <row r="253" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>2</v>
       </c>
@@ -23755,7 +23755,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="254" spans="1:28">
+    <row r="254" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>2</v>
       </c>
@@ -23841,7 +23841,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="255" spans="1:28">
+    <row r="255" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>2</v>
       </c>
@@ -23927,7 +23927,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="256" spans="1:28">
+    <row r="256" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>2</v>
       </c>
@@ -24013,7 +24013,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="257" spans="1:28">
+    <row r="257" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>2</v>
       </c>
@@ -24099,7 +24099,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="258" spans="1:28">
+    <row r="258" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>2</v>
       </c>
@@ -24185,7 +24185,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="259" spans="1:28">
+    <row r="259" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>2</v>
       </c>
@@ -24271,7 +24271,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="260" spans="1:28">
+    <row r="260" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>2</v>
       </c>
@@ -24357,7 +24357,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="261" spans="1:28">
+    <row r="261" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>2</v>
       </c>
@@ -24443,7 +24443,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="262" spans="1:28">
+    <row r="262" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>2</v>
       </c>
@@ -24529,7 +24529,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="263" spans="1:28">
+    <row r="263" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A263">
         <v>2</v>
       </c>
@@ -24615,7 +24615,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="264" spans="1:28">
+    <row r="264" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>2</v>
       </c>
@@ -24701,7 +24701,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="265" spans="1:28">
+    <row r="265" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>2</v>
       </c>
@@ -24787,7 +24787,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="266" spans="1:28">
+    <row r="266" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>2</v>
       </c>
@@ -24873,7 +24873,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="267" spans="1:28">
+    <row r="267" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>2</v>
       </c>
@@ -24959,7 +24959,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="268" spans="1:28">
+    <row r="268" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>2</v>
       </c>
@@ -25045,7 +25045,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="269" spans="1:28">
+    <row r="269" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>2</v>
       </c>
@@ -25131,7 +25131,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="270" spans="1:28">
+    <row r="270" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>2</v>
       </c>
@@ -25217,7 +25217,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="271" spans="1:28">
+    <row r="271" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>2</v>
       </c>
@@ -25303,7 +25303,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="272" spans="1:28">
+    <row r="272" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>2</v>
       </c>
@@ -25389,7 +25389,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="273" spans="1:28">
+    <row r="273" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>2</v>
       </c>
@@ -25475,7 +25475,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="274" spans="1:28">
+    <row r="274" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A274">
         <v>2</v>
       </c>
@@ -25561,7 +25561,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="275" spans="1:28">
+    <row r="275" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>2</v>
       </c>
@@ -25647,7 +25647,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="276" spans="1:28">
+    <row r="276" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A276">
         <v>2</v>
       </c>
@@ -25733,7 +25733,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="277" spans="1:28">
+    <row r="277" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A277">
         <v>2</v>
       </c>
@@ -25819,7 +25819,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="278" spans="1:28">
+    <row r="278" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>2</v>
       </c>
@@ -25905,7 +25905,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="279" spans="1:28">
+    <row r="279" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A279">
         <v>2</v>
       </c>
@@ -25991,7 +25991,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="280" spans="1:28">
+    <row r="280" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>2</v>
       </c>
@@ -26077,7 +26077,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="281" spans="1:28">
+    <row r="281" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A281">
         <v>2</v>
       </c>
@@ -26163,7 +26163,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="282" spans="1:28">
+    <row r="282" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>2</v>
       </c>
@@ -26249,7 +26249,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="283" spans="1:28">
+    <row r="283" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>2</v>
       </c>
@@ -26335,7 +26335,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="284" spans="1:28">
+    <row r="284" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>2</v>
       </c>
@@ -26421,7 +26421,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="285" spans="1:28">
+    <row r="285" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>2</v>
       </c>
@@ -26507,7 +26507,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="286" spans="1:28">
+    <row r="286" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>2</v>
       </c>
@@ -26593,7 +26593,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="287" spans="1:28">
+    <row r="287" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>2</v>
       </c>
@@ -26679,7 +26679,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="288" spans="1:28">
+    <row r="288" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>2</v>
       </c>
@@ -26765,7 +26765,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="289" spans="1:28">
+    <row r="289" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>2</v>
       </c>
@@ -26851,7 +26851,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="290" spans="1:28">
+    <row r="290" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>2</v>
       </c>
@@ -26937,7 +26937,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="291" spans="1:28">
+    <row r="291" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>2</v>
       </c>
@@ -27023,7 +27023,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="292" spans="1:28">
+    <row r="292" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>2</v>
       </c>
@@ -27109,7 +27109,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="293" spans="1:28">
+    <row r="293" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>2</v>
       </c>
@@ -27195,7 +27195,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="294" spans="1:28">
+    <row r="294" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>2</v>
       </c>
@@ -27281,7 +27281,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="295" spans="1:28">
+    <row r="295" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>2</v>
       </c>
@@ -27367,7 +27367,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="296" spans="1:28">
+    <row r="296" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>2</v>
       </c>
@@ -27453,7 +27453,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="297" spans="1:28">
+    <row r="297" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A297">
         <v>2</v>
       </c>
@@ -27539,7 +27539,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="298" spans="1:28">
+    <row r="298" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>2</v>
       </c>
@@ -27625,7 +27625,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="299" spans="1:28">
+    <row r="299" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>2</v>
       </c>
@@ -27711,7 +27711,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="300" spans="1:28">
+    <row r="300" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>2</v>
       </c>
@@ -27797,7 +27797,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="301" spans="1:28">
+    <row r="301" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>2</v>
       </c>
@@ -27883,7 +27883,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="302" spans="1:28">
+    <row r="302" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>2</v>
       </c>
@@ -27969,7 +27969,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="303" spans="1:28">
+    <row r="303" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A303">
         <v>2</v>
       </c>
@@ -28055,7 +28055,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="304" spans="1:28">
+    <row r="304" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A304">
         <v>2</v>
       </c>
@@ -28141,7 +28141,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="305" spans="1:28">
+    <row r="305" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A305">
         <v>2</v>
       </c>
@@ -28227,7 +28227,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="306" spans="1:28">
+    <row r="306" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A306">
         <v>2</v>
       </c>
@@ -28313,7 +28313,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="307" spans="1:28">
+    <row r="307" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A307">
         <v>2</v>
       </c>
@@ -28399,7 +28399,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="308" spans="1:28">
+    <row r="308" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A308">
         <v>2</v>
       </c>
@@ -28485,7 +28485,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="309" spans="1:28">
+    <row r="309" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A309">
         <v>2</v>
       </c>
@@ -28571,7 +28571,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="310" spans="1:28">
+    <row r="310" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A310">
         <v>2</v>
       </c>
@@ -28657,7 +28657,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="311" spans="1:28">
+    <row r="311" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A311">
         <v>2</v>
       </c>
@@ -28743,7 +28743,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="312" spans="1:28">
+    <row r="312" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A312">
         <v>2</v>
       </c>
@@ -28829,7 +28829,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="313" spans="1:28">
+    <row r="313" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A313">
         <v>2</v>
       </c>
@@ -28915,7 +28915,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="314" spans="1:28">
+    <row r="314" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A314">
         <v>2</v>
       </c>
@@ -29001,7 +29001,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="315" spans="1:28">
+    <row r="315" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A315">
         <v>2</v>
       </c>
@@ -29087,7 +29087,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="316" spans="1:28">
+    <row r="316" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A316">
         <v>2</v>
       </c>
@@ -29173,7 +29173,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="317" spans="1:28">
+    <row r="317" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A317">
         <v>2</v>
       </c>
@@ -29259,7 +29259,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="318" spans="1:28">
+    <row r="318" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A318">
         <v>2</v>
       </c>
@@ -29345,7 +29345,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="319" spans="1:28">
+    <row r="319" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A319">
         <v>2</v>
       </c>
@@ -29431,7 +29431,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="320" spans="1:28">
+    <row r="320" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A320">
         <v>2</v>
       </c>
@@ -29517,7 +29517,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="321" spans="1:28">
+    <row r="321" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A321">
         <v>2</v>
       </c>
@@ -29603,7 +29603,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="322" spans="1:28">
+    <row r="322" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A322">
         <v>2</v>
       </c>
@@ -29689,7 +29689,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="323" spans="1:28">
+    <row r="323" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A323">
         <v>2</v>
       </c>
@@ -29775,7 +29775,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="324" spans="1:28">
+    <row r="324" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A324">
         <v>2</v>
       </c>
@@ -29861,7 +29861,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="325" spans="1:28">
+    <row r="325" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A325">
         <v>2</v>
       </c>
@@ -29947,7 +29947,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="326" spans="1:28">
+    <row r="326" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A326">
         <v>2</v>
       </c>
@@ -30033,7 +30033,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="327" spans="1:28">
+    <row r="327" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A327">
         <v>2</v>
       </c>
@@ -30119,7 +30119,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="328" spans="1:28">
+    <row r="328" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A328">
         <v>2</v>
       </c>
@@ -30205,7 +30205,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="329" spans="1:28">
+    <row r="329" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A329">
         <v>2</v>
       </c>
@@ -30291,7 +30291,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="330" spans="1:28">
+    <row r="330" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A330">
         <v>2</v>
       </c>
@@ -30377,7 +30377,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="331" spans="1:28">
+    <row r="331" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A331">
         <v>2</v>
       </c>
@@ -30463,7 +30463,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="332" spans="1:28">
+    <row r="332" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A332">
         <v>2</v>
       </c>
@@ -30549,7 +30549,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="333" spans="1:28">
+    <row r="333" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A333">
         <v>2</v>
       </c>
@@ -30635,7 +30635,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="334" spans="1:28">
+    <row r="334" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A334">
         <v>2</v>
       </c>
@@ -30721,7 +30721,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="335" spans="1:28">
+    <row r="335" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A335">
         <v>2</v>
       </c>
@@ -30807,7 +30807,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="336" spans="1:28">
+    <row r="336" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A336">
         <v>2</v>
       </c>
@@ -30893,7 +30893,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="337" spans="1:28">
+    <row r="337" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A337">
         <v>2</v>
       </c>
@@ -30979,7 +30979,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="338" spans="1:28">
+    <row r="338" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A338">
         <v>2</v>
       </c>
@@ -31065,7 +31065,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="339" spans="1:28">
+    <row r="339" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A339">
         <v>2</v>
       </c>
@@ -31151,7 +31151,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="340" spans="1:28">
+    <row r="340" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A340">
         <v>2</v>
       </c>
@@ -31237,7 +31237,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="341" spans="1:28">
+    <row r="341" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A341">
         <v>2</v>
       </c>
@@ -31323,7 +31323,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="342" spans="1:28">
+    <row r="342" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A342">
         <v>2</v>
       </c>
@@ -31409,7 +31409,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="343" spans="1:28">
+    <row r="343" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A343">
         <v>2</v>
       </c>
@@ -31495,7 +31495,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="344" spans="1:28">
+    <row r="344" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A344">
         <v>2</v>
       </c>
@@ -31581,7 +31581,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="345" spans="1:28">
+    <row r="345" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A345">
         <v>2</v>
       </c>
@@ -31667,7 +31667,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="346" spans="1:28">
+    <row r="346" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A346">
         <v>2</v>
       </c>
@@ -31753,7 +31753,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="347" spans="1:28">
+    <row r="347" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A347">
         <v>2</v>
       </c>
@@ -31839,7 +31839,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="348" spans="1:28">
+    <row r="348" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A348">
         <v>2</v>
       </c>
@@ -31925,7 +31925,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="349" spans="1:28">
+    <row r="349" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A349">
         <v>2</v>
       </c>
@@ -32011,7 +32011,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="350" spans="1:28">
+    <row r="350" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A350">
         <v>2</v>
       </c>
@@ -32097,7 +32097,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="351" spans="1:28">
+    <row r="351" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A351">
         <v>2</v>
       </c>
@@ -32183,7 +32183,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="352" spans="1:28">
+    <row r="352" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A352">
         <v>2</v>
       </c>
@@ -32269,7 +32269,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="353" spans="1:28">
+    <row r="353" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A353">
         <v>2</v>
       </c>
@@ -32355,7 +32355,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="354" spans="1:28">
+    <row r="354" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A354">
         <v>2</v>
       </c>
@@ -32441,7 +32441,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="355" spans="1:28">
+    <row r="355" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A355">
         <v>2</v>
       </c>
@@ -32527,7 +32527,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="356" spans="1:28">
+    <row r="356" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A356">
         <v>2</v>
       </c>
@@ -32613,7 +32613,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="357" spans="1:28">
+    <row r="357" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A357">
         <v>2</v>
       </c>
@@ -32699,7 +32699,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="358" spans="1:28">
+    <row r="358" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A358">
         <v>2</v>
       </c>
@@ -32785,7 +32785,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="359" spans="1:28">
+    <row r="359" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A359">
         <v>2</v>
       </c>
@@ -32871,7 +32871,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="360" spans="1:28">
+    <row r="360" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A360">
         <v>2</v>
       </c>
@@ -32957,7 +32957,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="361" spans="1:28">
+    <row r="361" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A361">
         <v>2</v>
       </c>
@@ -33043,7 +33043,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="362" spans="1:28">
+    <row r="362" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A362">
         <v>2</v>
       </c>
@@ -33129,7 +33129,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="363" spans="1:28">
+    <row r="363" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A363">
         <v>2</v>
       </c>
@@ -33215,7 +33215,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="364" spans="1:28">
+    <row r="364" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A364">
         <v>2</v>
       </c>
@@ -33301,7 +33301,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="365" spans="1:28">
+    <row r="365" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A365">
         <v>2</v>
       </c>
@@ -33387,7 +33387,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="366" spans="1:28">
+    <row r="366" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A366">
         <v>2</v>
       </c>
@@ -33473,7 +33473,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="367" spans="1:28">
+    <row r="367" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A367">
         <v>2</v>
       </c>
@@ -33559,7 +33559,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="368" spans="1:28">
+    <row r="368" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A368">
         <v>2</v>
       </c>
@@ -33645,7 +33645,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="369" spans="1:28">
+    <row r="369" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A369">
         <v>2</v>
       </c>
@@ -33731,7 +33731,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="370" spans="1:28">
+    <row r="370" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A370">
         <v>2</v>
       </c>
@@ -33817,7 +33817,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="371" spans="1:28">
+    <row r="371" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A371">
         <v>2</v>
       </c>
@@ -33903,7 +33903,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="372" spans="1:28">
+    <row r="372" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A372">
         <v>2</v>
       </c>
@@ -33989,7 +33989,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="373" spans="1:28">
+    <row r="373" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A373">
         <v>2</v>
       </c>
@@ -34075,7 +34075,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="374" spans="1:28">
+    <row r="374" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A374">
         <v>2</v>
       </c>
@@ -34161,7 +34161,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="375" spans="1:28">
+    <row r="375" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A375">
         <v>2</v>
       </c>
@@ -34247,7 +34247,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="376" spans="1:28">
+    <row r="376" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A376">
         <v>2</v>
       </c>
@@ -34333,7 +34333,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="377" spans="1:28">
+    <row r="377" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A377">
         <v>2</v>
       </c>
@@ -34419,7 +34419,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="378" spans="1:28">
+    <row r="378" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A378">
         <v>2</v>
       </c>
@@ -34505,7 +34505,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="379" spans="1:28">
+    <row r="379" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A379">
         <v>2</v>
       </c>
@@ -34591,7 +34591,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="380" spans="1:28">
+    <row r="380" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A380">
         <v>2</v>
       </c>
@@ -34677,7 +34677,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="381" spans="1:28">
+    <row r="381" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A381">
         <v>2</v>
       </c>
@@ -34763,7 +34763,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="382" spans="1:28">
+    <row r="382" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A382">
         <v>2</v>
       </c>
@@ -34849,7 +34849,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="383" spans="1:28">
+    <row r="383" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A383">
         <v>2</v>
       </c>
@@ -34935,7 +34935,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="384" spans="1:28">
+    <row r="384" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A384">
         <v>2</v>
       </c>
@@ -35021,7 +35021,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="385" spans="1:28">
+    <row r="385" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A385">
         <v>2</v>
       </c>
@@ -35107,7 +35107,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="386" spans="1:28">
+    <row r="386" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A386">
         <v>2</v>
       </c>
@@ -35193,7 +35193,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="387" spans="1:28">
+    <row r="387" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A387">
         <v>2</v>
       </c>
@@ -35279,7 +35279,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="388" spans="1:28">
+    <row r="388" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A388">
         <v>2</v>
       </c>
@@ -35365,7 +35365,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="389" spans="1:28">
+    <row r="389" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A389">
         <v>2</v>
       </c>
@@ -35451,7 +35451,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="390" spans="1:28">
+    <row r="390" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A390">
         <v>2</v>
       </c>
@@ -35537,7 +35537,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="391" spans="1:28">
+    <row r="391" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A391">
         <v>2</v>
       </c>
@@ -35623,7 +35623,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="392" spans="1:28">
+    <row r="392" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A392">
         <v>2</v>
       </c>
@@ -35709,7 +35709,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="393" spans="1:28">
+    <row r="393" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A393">
         <v>2</v>
       </c>
@@ -35795,7 +35795,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="394" spans="1:28">
+    <row r="394" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A394">
         <v>2</v>
       </c>
@@ -35881,7 +35881,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="395" spans="1:28">
+    <row r="395" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A395">
         <v>2</v>
       </c>
@@ -35967,7 +35967,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="396" spans="1:28">
+    <row r="396" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A396">
         <v>2</v>
       </c>
@@ -36053,7 +36053,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="397" spans="1:28">
+    <row r="397" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A397">
         <v>2</v>
       </c>
@@ -36139,7 +36139,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="398" spans="1:28">
+    <row r="398" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A398">
         <v>2</v>
       </c>
@@ -36225,7 +36225,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="399" spans="1:28">
+    <row r="399" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A399">
         <v>2</v>
       </c>
@@ -36311,7 +36311,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="400" spans="1:28">
+    <row r="400" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A400">
         <v>2</v>
       </c>
@@ -36397,7 +36397,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="401" spans="1:28">
+    <row r="401" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A401">
         <v>2</v>
       </c>
@@ -36483,7 +36483,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="402" spans="1:28">
+    <row r="402" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A402">
         <v>2</v>
       </c>
@@ -36569,7 +36569,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="403" spans="1:28">
+    <row r="403" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A403">
         <v>2</v>
       </c>
@@ -36655,7 +36655,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="404" spans="1:28">
+    <row r="404" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A404">
         <v>2</v>
       </c>
@@ -36741,7 +36741,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="405" spans="1:28">
+    <row r="405" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A405">
         <v>2</v>
       </c>
@@ -36827,7 +36827,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="406" spans="1:28">
+    <row r="406" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A406">
         <v>2</v>
       </c>
@@ -36913,7 +36913,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="407" spans="1:28">
+    <row r="407" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A407">
         <v>2</v>
       </c>
@@ -36999,7 +36999,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="408" spans="1:28">
+    <row r="408" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A408">
         <v>2</v>
       </c>
@@ -37085,7 +37085,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="409" spans="1:28">
+    <row r="409" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A409">
         <v>2</v>
       </c>
@@ -37171,7 +37171,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="410" spans="1:28">
+    <row r="410" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A410">
         <v>2</v>
       </c>
@@ -37257,7 +37257,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="411" spans="1:28">
+    <row r="411" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A411">
         <v>2</v>
       </c>
@@ -37343,7 +37343,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="412" spans="1:28">
+    <row r="412" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A412">
         <v>2</v>
       </c>
@@ -37429,7 +37429,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="413" spans="1:28">
+    <row r="413" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A413">
         <v>2</v>
       </c>
@@ -37515,7 +37515,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="414" spans="1:28">
+    <row r="414" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A414">
         <v>2</v>
       </c>
@@ -37601,7 +37601,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="415" spans="1:28">
+    <row r="415" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A415">
         <v>2</v>
       </c>
@@ -37688,26 +37688,25 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AB415" xr:uid="{587186FB-6F3F-4979-808F-38B12FBAB3C5}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <File xmlns="3d137487-0b15-4ad9-abee-bf6b36a5a6e0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <File xmlns="3d137487-0b15-4ad9-abee-bf6b36a5a6e0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -37934,13 +37933,38 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7274625E-67DB-4651-897C-6D7DC66B68D7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08A3BD12-C07C-45D6-A144-898F8A53501B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08A3BD12-C07C-45D6-A144-898F8A53501B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7274625E-67DB-4651-897C-6D7DC66B68D7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3d137487-0b15-4ad9-abee-bf6b36a5a6e0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E89494C-5618-4A40-A709-21FDFFDAB717}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E89494C-5618-4A40-A709-21FDFFDAB717}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3d137487-0b15-4ad9-abee-bf6b36a5a6e0"/>
+    <ds:schemaRef ds:uri="81cf108f-c583-47b3-8493-b6de3c823d22"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>